<commit_message>
Using dbt to add the fact table for real estate data
</commit_message>
<xml_diff>
--- a/data/real_estate_listings.xlsx
+++ b/data/real_estate_listings.xlsx
@@ -1743,7 +1743,7 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t>['https://file4.batdongsan.com.vn/crop/232x186/2025/11/14/20251114210543-de01_wm.jpg', 'https://file4.batdongsan.com.vn/crop/115x64/2025/11/14/20251114210815-b339_wm.jpg', 'https://file4.batdongsan.com.vn/crop/115x64/2025/11/14/20251114210816-d27d_wm.jpg', 'https://file4.batdongsan.com.vn/resize/200x200/2025/09/04/20250904155050-3b73.jpg']</t>
+          <t>['https://file4.batdongsan.com.vn/resize/200x200/2025/09/04/20250904155050-3b73.jpg']</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2117,7 +2117,7 @@
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
-          <t>['https://file4.batdongsan.com.vn/crop/232x186/2026/01/05/20260105100911-8bdc_wm.jpg', 'https://staticfile.batdongsan.com.vn/images/Product/expired_icon.svg']</t>
+          <t>['https://staticfile.batdongsan.com.vn/images/Product/expired_icon.svg']</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2180,7 +2180,7 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>['https://file4.batdongsan.com.vn/crop/232x186/2025/12/31/20251231164307-2624_wm.jpg', 'https://staticfile.batdongsan.com.vn/images/Product/expired_icon.svg']</t>
+          <t>['https://staticfile.batdongsan.com.vn/images/Product/expired_icon.svg']</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2243,7 +2243,7 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t>['https://file4.batdongsan.com.vn/crop/232x186/2025/12/27/20251227203753-a90e_wm.jpg', 'https://staticfile.batdongsan.com.vn/images/Product/expired_icon.svg']</t>
+          <t>['https://staticfile.batdongsan.com.vn/images/Product/expired_icon.svg']</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2924,7 +2924,7 @@
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
         <is>
-          <t>['https://file4.batdongsan.com.vn/crop/232x186/2026/02/05/20260205110214-0569_wm.jpg', 'https://staticfile.batdongsan.com.vn/images/Product/expired_icon.svg', 'https://file4.batdongsan.com.vn/resize/200x200/2024/10/24/20241024154638-4995.jpg']</t>
+          <t>['https://staticfile.batdongsan.com.vn/images/Product/expired_icon.svg', 'https://file4.batdongsan.com.vn/resize/200x200/2024/10/24/20241024154638-4995.jpg']</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">

</xml_diff>